<commit_message>
feat: add more statistics + refactor
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26827"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Konstantin Papirnik\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\chris\PycharmProjects\BA1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{326F00C5-B253-476B-A56A-CA57859C8BC8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B9379A47-72DC-47E5-A22B-116F621B567E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="38280" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabellenblatt1" sheetId="1" r:id="rId1"/>
@@ -285,7 +285,7 @@
     <xf numFmtId="165" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Standard" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="3">
     <dxf>
@@ -530,10 +530,10 @@
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="Y9" sqref="Y9"/>
+      <selection pane="bottomLeft" activeCell="X2" sqref="X2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="11.6640625" customWidth="1"/>
     <col min="2" max="2" width="8.33203125" customWidth="1"/>
@@ -23618,7 +23618,7 @@
       <c r="Y324" s="1"/>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="X1:X854 Y1">
+  <conditionalFormatting sqref="Y1 X1:X854">
     <cfRule type="beginsWith" dxfId="2" priority="1" operator="beginsWith" text="W">
       <formula>LEFT((X1),LEN("W"))=("W")</formula>
     </cfRule>

</xml_diff>